<commit_message>
user koppe zwischen commit
git-svn-id: http://svn.code.sf.net/p/segelboot/code@497 2e2d5edc-86b9-48e7-b817-bf6befc431f3
</commit_message>
<xml_diff>
--- a/trunk/sairo_rudderpos_compasscourse_compare.xlsx
+++ b/trunk/sairo_rudderpos_compasscourse_compare.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="23715" windowHeight="10035" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="23715" windowHeight="9975" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="sairo_rudderposList" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="sairo_compasscourseslist" localSheetId="0">sairo_rudderposList!$A$1249:$B$2023</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -18431,11 +18431,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="57260288"/>
-        <c:axId val="61106048"/>
+        <c:axId val="88204800"/>
+        <c:axId val="88206336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="57260288"/>
+        <c:axId val="88204800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18444,7 +18444,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61106048"/>
+        <c:crossAx val="88206336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18452,7 +18452,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61106048"/>
+        <c:axId val="88206336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18463,14 +18463,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57260288"/>
+        <c:crossAx val="88204800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -33962,11 +33961,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="58254848"/>
-        <c:axId val="58256384"/>
+        <c:axId val="89907968"/>
+        <c:axId val="89909504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="58254848"/>
+        <c:axId val="89907968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -33975,7 +33974,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="58256384"/>
+        <c:crossAx val="89909504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -33983,7 +33982,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58256384"/>
+        <c:axId val="89909504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -33994,7 +33993,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58254848"/>
+        <c:crossAx val="89907968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>